<commit_message>
update load course from csv
</commit_message>
<xml_diff>
--- a/Savefile/SchoolYear/2021-2022/Course/Course.xlsx
+++ b/Savefile/SchoolYear/2021-2022/Course/Course.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -335,7 +335,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>